<commit_message>
adding after 12 changes
</commit_message>
<xml_diff>
--- a/pick_counts.xlsx
+++ b/pick_counts.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,23 +470,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C2" t="n">
-        <v>5.876288659793814</v>
+        <v>13.98963730569948</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>2.474226804123711</v>
+        <v>8.393782383419689</v>
       </c>
     </row>
     <row r="4">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>255</v>
+        <v>161</v>
       </c>
       <c r="C4" t="n">
-        <v>78.8659793814433</v>
+        <v>50.05181347150259</v>
       </c>
     </row>
     <row r="5">
@@ -509,205 +509,101 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>209</v>
+        <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>64.63917525773196</v>
+        <v>8.393782383419689</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C6" t="n">
-        <v>8.659793814432989</v>
+        <v>14.92227979274611</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C7" t="n">
-        <v>1.54639175257732</v>
+        <v>16.16580310880829</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>3.711340206185567</v>
+        <v>0.6217616580310881</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2</v>
+        <v>99</v>
       </c>
       <c r="C9" t="n">
-        <v>0.6185567010309279</v>
+        <v>30.77720207253886</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="C10" t="n">
-        <v>23.81443298969072</v>
+        <v>32.95336787564766</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C11" t="n">
-        <v>2.783505154639175</v>
+        <v>7.150259067357513</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>66</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>20.41237113402062</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>PATR5027.AMEH</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>71</v>
-      </c>
-      <c r="C13" t="n">
-        <v>21.95876288659794</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>RAMI9087.SAIHI</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>173</v>
-      </c>
-      <c r="C14" t="n">
-        <v>53.50515463917526</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>117</v>
-      </c>
-      <c r="C15" t="n">
-        <v>36.18556701030928</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>TAMISHA.DAVY</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>123</v>
-      </c>
-      <c r="C16" t="n">
-        <v>38.04123711340206</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>TANI2739.HOSSAINISLA</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>242</v>
-      </c>
-      <c r="C17" t="n">
-        <v>74.84536082474227</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>165</v>
-      </c>
-      <c r="C18" t="n">
-        <v>51.03092783505154</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>XYZE1559.MACASIL</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>58</v>
-      </c>
-      <c r="C19" t="n">
-        <v>17.93814432989691</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>5</v>
-      </c>
-      <c r="C20" t="n">
-        <v>1.54639175257732</v>
+        <v>1.55440414507772</v>
       </c>
     </row>
   </sheetData>
@@ -749,66 +645,66 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BOHD0676.KUSHLIAK</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4.329896907216495</v>
+        <v>0.310880829015544</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>11.44329896907217</v>
+        <v>2.797927461139896</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C4" t="n">
-        <v>0.3092783505154639</v>
+        <v>16.78756476683938</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>2.164948453608247</v>
+        <v>2.487046632124352</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>2.783505154639175</v>
+        <v>1.243523316062176</v>
       </c>
     </row>
     <row r="7">
@@ -818,23 +714,23 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
-        <v>0.9278350515463918</v>
+        <v>9.326424870466321</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>4</v>
       </c>
       <c r="C8" t="n">
-        <v>1.237113402061856</v>
+        <v>1.243523316062176</v>
       </c>
     </row>
   </sheetData>
@@ -848,7 +744,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -876,79 +772,92 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>5.876288659793814</v>
+        <v>10.88082901554404</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C3" t="n">
-        <v>4.020618556701031</v>
+        <v>4.352331606217616</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>13</v>
+        <v>50</v>
       </c>
       <c r="C4" t="n">
-        <v>4.020618556701031</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>TAMISHA.DAVY</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>25</v>
+        <v>153</v>
       </c>
       <c r="C5" t="n">
-        <v>7.731958762886598</v>
+        <v>47.56476683937824</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>66</v>
+        <v>86</v>
       </c>
       <c r="C6" t="n">
-        <v>20.41237113402062</v>
+        <v>26.73575129533679</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>6.804123711340206</v>
+        <v>3.730569948186528</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>15</v>
+      </c>
+      <c r="C8" t="n">
+        <v>4.66321243523316</v>
       </c>
     </row>
   </sheetData>
@@ -962,7 +871,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -990,235 +899,300 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AHME0710.JUBRAN</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>170</v>
       </c>
       <c r="C2" t="n">
-        <v>3.092783505154639</v>
+        <v>52.84974093264248</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>21.34020618556701</v>
+        <v>25.49222797927461</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BUDD0680.TENNAKOON</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="C4" t="n">
-        <v>18.24742268041237</v>
+        <v>7.150259067357513</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>BUDD0680.TENNAKOON</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="C5" t="n">
-        <v>18.8659793814433</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C6" t="n">
-        <v>25.67010309278351</v>
+        <v>27.04663212435233</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="C7" t="n">
-        <v>12.37113402061856</v>
+        <v>28.29015544041451</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="C8" t="n">
-        <v>24.74226804123711</v>
+        <v>22.69430051813471</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MARI882N.ABDELKADER</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>96</v>
       </c>
       <c r="C9" t="n">
-        <v>0.9278350515463918</v>
+        <v>29.84455958549223</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>120</v>
+        <v>84</v>
       </c>
       <c r="C10" t="n">
-        <v>37.11340206185567</v>
+        <v>26.1139896373057</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="C11" t="n">
-        <v>32.47422680412371</v>
+        <v>15.5440414507772</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C12" t="n">
-        <v>8.350515463917526</v>
+        <v>17.72020725388601</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>123</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>38.04123711340206</v>
+        <v>11.50259067357513</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>REJWAN.ISLAM</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>74</v>
+        <v>103</v>
       </c>
       <c r="C14" t="n">
-        <v>22.88659793814433</v>
+        <v>32.02072538860104</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>STAN9294.BAUER</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>25</v>
+        <v>76</v>
       </c>
       <c r="C15" t="n">
-        <v>7.731958762886598</v>
+        <v>23.62694300518135</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SURESH.DHAWAN</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="C16" t="n">
-        <v>38.65979381443299</v>
+        <v>18.96373056994819</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="C17" t="n">
-        <v>20.72164948453608</v>
+        <v>31.39896373056995</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>176</v>
+        <v>33</v>
       </c>
       <c r="C18" t="n">
-        <v>54.43298969072165</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C19" t="n">
-        <v>19.48453608247423</v>
+        <v>26.42487046632124</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>TUSHAR.BHATIA</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>99</v>
+      </c>
+      <c r="C20" t="n">
+        <v>30.77720207253886</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>WESL5337.CADETTE</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>83</v>
+      </c>
+      <c r="C21" t="n">
+        <v>25.80310880829015</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>WILDINE.JEUNE</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>172</v>
+      </c>
+      <c r="C22" t="n">
+        <v>53.47150259067357</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>YATI0689.YATIN</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>112</v>
+      </c>
+      <c r="C23" t="n">
+        <v>34.81865284974093</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>ZAKI0190.PHILLIPHORS</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>118</v>
+      </c>
+      <c r="C24" t="n">
+        <v>36.68393782383419</v>
       </c>
     </row>
   </sheetData>
@@ -1232,7 +1206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1260,261 +1234,170 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AGNE8120.CARUTH</t>
+          <t>ADOL798N.SEEMANNVAZQ</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="C2" t="n">
-        <v>20.72164948453608</v>
+        <v>53.78238341968912</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ALMER.VILLAMIN</t>
+          <t>BOHD0676.KUSHLIAK</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>79</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3092783505154639</v>
+        <v>24.55958549222798</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C4" t="n">
-        <v>8.969072164948454</v>
+        <v>10.25906735751295</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>379</v>
+        <v>154</v>
       </c>
       <c r="C5" t="n">
-        <v>117.2164948453608</v>
+        <v>47.87564766839378</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>66</v>
+        <v>321</v>
       </c>
       <c r="C6" t="n">
-        <v>20.41237113402062</v>
+        <v>99.79274611398964</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3092783505154639</v>
+        <v>3.10880829015544</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>31</v>
+        <v>171</v>
       </c>
       <c r="C8" t="n">
-        <v>9.587628865979381</v>
+        <v>53.16062176165803</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MAKEDA.OLLIVIERRE</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C9" t="n">
-        <v>16.39175257731959</v>
+        <v>30.15544041450777</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>STAN9294.BAUER</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C10" t="n">
-        <v>3.402061855670103</v>
+        <v>34.81865284974093</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>SURESH.DHAWAN</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>73</v>
+        <v>199</v>
       </c>
       <c r="C11" t="n">
-        <v>22.57731958762886</v>
+        <v>61.86528497409326</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>215</v>
+        <v>86</v>
       </c>
       <c r="C12" t="n">
-        <v>66.49484536082474</v>
+        <v>26.73575129533679</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>30</v>
+        <v>107</v>
       </c>
       <c r="C13" t="n">
-        <v>9.278350515463917</v>
+        <v>33.26424870466321</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>107</v>
+        <v>42</v>
       </c>
       <c r="C14" t="n">
-        <v>33.09278350515464</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>RAMI9087.SAIHI</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>110</v>
-      </c>
-      <c r="C15" t="n">
-        <v>34.02061855670103</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>RARG046N.YEBOAH</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>90</v>
-      </c>
-      <c r="C16" t="n">
-        <v>27.83505154639175</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>STAN9294.BAUER</t>
-        </is>
-      </c>
-      <c r="B17" t="n">
-        <v>56</v>
-      </c>
-      <c r="C17" t="n">
-        <v>17.31958762886598</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>SURESH.DHAWAN</t>
-        </is>
-      </c>
-      <c r="B18" t="n">
-        <v>37</v>
-      </c>
-      <c r="C18" t="n">
-        <v>11.44329896907217</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>TAMISHA.DAVY</t>
-        </is>
-      </c>
-      <c r="B19" t="n">
-        <v>80</v>
-      </c>
-      <c r="C19" t="n">
-        <v>24.74226804123711</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>THIE6554.DIALLO</t>
-        </is>
-      </c>
-      <c r="B20" t="n">
-        <v>202</v>
-      </c>
-      <c r="C20" t="n">
-        <v>62.47422680412371</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>XYZE1559.MACASIL</t>
-        </is>
-      </c>
-      <c r="B21" t="n">
-        <v>22</v>
-      </c>
-      <c r="C21" t="n">
-        <v>6.804123711340206</v>
+        <v>13.05699481865285</v>
       </c>
     </row>
   </sheetData>
@@ -1528,7 +1411,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1555,27 +1438,27 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ALMER.VILLAMIN</t>
+          <t>AGNE8120.CARUTH</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>90</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ANJALI.BAKSHI</t>
+          <t>ARJUNBHAI.PATEL</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>114</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5">
@@ -1585,7 +1468,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>35</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6">
@@ -1595,157 +1478,157 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>135</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DIAN4065.ENTRIALGO</t>
+          <t>DEVI789.SINGH</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESSE0616.UDEH</t>
+          <t>DIAN4065.ENTRIALGO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IREN797N.CABRERA</t>
+          <t>ESSE0616.UDEH</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>63</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JEEW9554.SITUMUDALIG</t>
+          <t>GIGNESH.PATEL</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>33</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>KHINEHAYMAR.THAUNG</t>
+          <t>INUK4091.QAVAVAU</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>174</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>LOANA.MBONGO</t>
+          <t>JEEW9554.SITUMUDALIG</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>LOWRHY-OTIENO.JAOKO</t>
+          <t>KADE3054.ZONGO</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>93</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MELA6559.ROCHETTE</t>
+          <t>LOANA.MBONGO</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>161</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MICA0432.RIZKALLAMAR</t>
+          <t>MARI882N.ABDELKADER</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>84</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NESR2403.ATTALAH</t>
+          <t>MICA0432.RIZKALLAMAR</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>59</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>PATI2298.ATSIANGBE</t>
+          <t>NESR2403.ATTALAH</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>87</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>PATR5027.AMEH</t>
+          <t>OMAR6689.KHAN</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>98</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>RAMI9087.SAIHI</t>
+          <t>PATR5027.AMEH</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>45</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>RARG046N.YEBOAH</t>
+          <t>PRINCE.FORSON</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>31</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>REJWAN.ISLAM</t>
+          <t>SEPIDEH.AZARIHASHJIN</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>86</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
@@ -1755,7 +1638,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
@@ -1765,13 +1648,13 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>80</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>TAMISHA.DAVY</t>
+          <t>THIE6554.DIALLO</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1781,71 +1664,61 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>TANI2739.HOSSAINISLA</t>
+          <t>TUSHAR.BHATIA</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>THIE6554.DIALLO</t>
+          <t>WESL5337.CADETTE</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>WESL5337.CADETTE</t>
+          <t>WILDINE.JEUNE</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>75</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>WILDINE.JEUNE</t>
+          <t>YATI0689.YATIN</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>XYZE1559.MACASIL</t>
+          <t>ZAHIDGUL.MINHAS</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>164</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ZAHIDGUL.MINHAS</t>
+          <t>ZAKI0190.PHILLIPHORS</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>ZAKI0190.PHILLIPHORS</t>
-        </is>
-      </c>
-      <c r="B31" t="n">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -1859,7 +1732,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1896,157 +1769,89 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-2</v>
+        <v>-27</v>
       </c>
       <c r="C2" t="n">
-        <v>-25</v>
+        <v>-24</v>
       </c>
       <c r="D2" t="n">
-        <v>-222</v>
+        <v>-468</v>
       </c>
       <c r="E2" t="n">
-        <v>-220</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-5</v>
+        <v>-41</v>
       </c>
       <c r="C3" t="n">
-        <v>-125</v>
+        <v>-130</v>
       </c>
       <c r="D3" t="n">
-        <v>-521</v>
+        <v>-788</v>
       </c>
       <c r="E3" t="n">
-        <v>-827</v>
+        <v>-81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-58</v>
+        <v>-32</v>
       </c>
       <c r="C4" t="n">
-        <v>-8</v>
+        <v>-168</v>
       </c>
       <c r="D4" t="n">
-        <v>-426</v>
+        <v>-645</v>
       </c>
       <c r="E4" t="n">
-        <v>-458</v>
+        <v>-357</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="B5" t="n">
         <v>-10</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>-43</v>
       </c>
       <c r="D5" t="n">
-        <v>-141</v>
+        <v>-104</v>
       </c>
       <c r="E5" t="n">
-        <v>-139</v>
+        <v>-156</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>-110</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>-365</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>-2005</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="n">
-        <v>0</v>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="B10" t="n">
-        <v>-75</v>
-      </c>
-      <c r="C10" t="n">
-        <v>-158</v>
-      </c>
-      <c r="D10" t="n">
-        <v>-1310</v>
-      </c>
-      <c r="E10" t="n">
-        <v>-1644</v>
+        <v>-595</v>
       </c>
     </row>
   </sheetData>

</xml_diff>